<commit_message>
Plots and first conclusions
</commit_message>
<xml_diff>
--- a/canciones_bb_filled.xlsx
+++ b/canciones_bb_filled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/12822d402b62d09b/Documentos/Universidad/Data/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{D4F9D882-1CB0-4271-81DF-3649987B594F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{88961FD9-EEA3-431E-9FD5-8CEB3E4F55D7}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{D4F9D882-1CB0-4271-81DF-3649987B594F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CDFAAEC9-1FC4-4358-A126-2E9DA2F30C0B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="215">
   <si>
     <t>track_name</t>
   </si>
@@ -403,9 +403,6 @@
     <t>PERRO NEGRO</t>
   </si>
   <si>
-    <t>EUROPA :(</t>
-  </si>
-  <si>
     <t>ACHO PR</t>
   </si>
   <si>
@@ -662,6 +659,12 @@
   </si>
   <si>
     <t>is_reggaeton</t>
+  </si>
+  <si>
+    <t>El Favorito de los Capo (Remix)</t>
+  </si>
+  <si>
+    <t>EUROPA :)</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B213"/>
+  <dimension ref="A1:B214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1044,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2054,7 +2057,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>214</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -2062,7 +2065,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -2070,7 +2073,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -2078,7 +2081,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -2086,7 +2089,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -2094,7 +2097,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -2102,7 +2105,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -2110,7 +2113,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -2118,7 +2121,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -2126,7 +2129,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -2134,7 +2137,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -2142,7 +2145,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -2150,7 +2153,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -2158,7 +2161,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -2166,7 +2169,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2174,7 +2177,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -2182,7 +2185,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -2190,7 +2193,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -2198,7 +2201,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -2206,7 +2209,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -2214,7 +2217,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -2222,7 +2225,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -2230,7 +2233,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -2238,7 +2241,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B151">
         <v>1</v>
@@ -2246,7 +2249,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B152">
         <v>1</v>
@@ -2254,7 +2257,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -2262,7 +2265,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -2270,7 +2273,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -2278,7 +2281,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -2286,7 +2289,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -2294,7 +2297,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -2302,7 +2305,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -2310,7 +2313,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -2318,7 +2321,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -2326,7 +2329,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -2334,7 +2337,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -2342,7 +2345,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -2350,7 +2353,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B165">
         <v>1</v>
@@ -2358,7 +2361,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B166">
         <v>1</v>
@@ -2366,7 +2369,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -2374,7 +2377,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -2382,7 +2385,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -2390,7 +2393,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B170">
         <v>1</v>
@@ -2398,7 +2401,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -2406,7 +2409,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -2414,7 +2417,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -2422,7 +2425,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -2430,7 +2433,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -2438,7 +2441,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -2446,7 +2449,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B177">
         <v>1</v>
@@ -2454,7 +2457,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -2462,7 +2465,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B179">
         <v>1</v>
@@ -2470,7 +2473,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -2478,7 +2481,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B181">
         <v>1</v>
@@ -2486,7 +2489,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B182">
         <v>1</v>
@@ -2494,7 +2497,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B183">
         <v>1</v>
@@ -2502,7 +2505,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B184">
         <v>1</v>
@@ -2510,7 +2513,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B185">
         <v>1</v>
@@ -2518,7 +2521,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B186">
         <v>1</v>
@@ -2526,7 +2529,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B187">
         <v>1</v>
@@ -2534,7 +2537,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B188">
         <v>1</v>
@@ -2542,7 +2545,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B189">
         <v>1</v>
@@ -2550,7 +2553,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B190">
         <v>1</v>
@@ -2558,7 +2561,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -2566,7 +2569,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -2574,7 +2577,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -2582,7 +2585,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -2590,7 +2593,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -2598,7 +2601,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -2606,7 +2609,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -2614,7 +2617,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -2622,7 +2625,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B199">
         <v>1</v>
@@ -2630,7 +2633,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -2638,7 +2641,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B201">
         <v>0</v>
@@ -2646,7 +2649,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -2654,7 +2657,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -2662,7 +2665,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B204">
         <v>1</v>
@@ -2670,7 +2673,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B205">
         <v>0</v>
@@ -2678,7 +2681,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B206">
         <v>0</v>
@@ -2686,7 +2689,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B207">
         <v>1</v>
@@ -2694,7 +2697,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B208">
         <v>1</v>
@@ -2702,7 +2705,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B209">
         <v>1</v>
@@ -2710,7 +2713,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B210">
         <v>0</v>
@@ -2718,7 +2721,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B211">
         <v>0</v>
@@ -2726,7 +2729,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B212">
         <v>1</v>
@@ -2734,9 +2737,17 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>213</v>
+      </c>
+      <c r="B214">
         <v>0</v>
       </c>
     </row>

</xml_diff>